<commit_message>
added melody object it's soo pretty :)))
</commit_message>
<xml_diff>
--- a/markov.xlsx
+++ b/markov.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24426"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1600" windowWidth="24000" windowHeight="9740"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -54,13 +56,13 @@
     <t>Fmaj7</t>
   </si>
   <si>
-    <t>C/E</t>
+    <t>Sum</t>
   </si>
   <si>
     <t>Dm7</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Cmaj7</t>
   </si>
 </sst>
 </file>
@@ -168,7 +170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -203,7 +205,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,7 +382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,15 +393,12 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -422,7 +421,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -436,14 +435,16 @@
       <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -452,19 +453,19 @@
         <v>5</v>
       </c>
       <c r="E2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2">
         <v>27</v>
       </c>
       <c r="G2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <v>6</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -478,8 +479,12 @@
       <c r="M2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="N2">
+        <f>SUM(B2:M2)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -487,7 +492,7 @@
         <v>15</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -496,16 +501,16 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>3</v>
@@ -519,8 +524,12 @@
       <c r="M3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="N3">
+        <f t="shared" ref="N3:N13" si="0">SUM(B3:M3)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,10 +537,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4">
         <v>33</v>
@@ -560,8 +569,12 @@
       <c r="M4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -575,13 +588,13 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5">
         <v>28</v>
       </c>
       <c r="G5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -601,8 +614,12 @@
       <c r="M5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -613,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>24</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <v>26</v>
@@ -642,8 +659,12 @@
       <c r="M6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -654,7 +675,7 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <v>27</v>
@@ -663,7 +684,7 @@
         <v>26</v>
       </c>
       <c r="G7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H7">
         <v>6</v>
@@ -683,8 +704,12 @@
       <c r="M7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -707,10 +732,10 @@
         <v>31</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -724,49 +749,57 @@
       <c r="M8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>14</v>
-      </c>
-      <c r="C9">
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9">
         <v>11</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>36</v>
-      </c>
-      <c r="F9">
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
         <v>12</v>
       </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>5</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>10</v>
-      </c>
       <c r="L9">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="M9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>22</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -792,22 +825,26 @@
         <v>2</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L10">
         <v>17</v>
       </c>
       <c r="M10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>16</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -821,10 +858,10 @@
         <v>4</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F11">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G11">
         <v>6</v>
@@ -833,22 +870,26 @@
         <v>2</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J11">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L11">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>8</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -874,7 +915,7 @@
         <v>3</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <v>11</v>
@@ -883,13 +924,17 @@
         <v>15</v>
       </c>
       <c r="L12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -915,7 +960,7 @@
         <v>3</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13">
         <v>17</v>
@@ -927,16 +972,15 @@
         <v>4</v>
       </c>
       <c r="M13">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>